<commit_message>
finished no register order test
finished no register order test
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TESTY\online_store_selenium\untitled\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C2E0EA-DD76-4977-A1E0-7C9406BA866E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3316F27B-46A5-40EA-8907-7920AB0D5DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="396" windowWidth="23040" windowHeight="11964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="home page product list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
   <si>
     <t>Rampers niemowlęcy na zamek, rakiety</t>
   </si>
@@ -170,15 +170,6 @@
     <t>city</t>
   </si>
   <si>
-    <t xml:space="preserve">Kataryna </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anna </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria </t>
-  </si>
-  <si>
     <t>Leona</t>
   </si>
   <si>
@@ -188,9 +179,6 @@
     <t>Ludmiła</t>
   </si>
   <si>
-    <t xml:space="preserve">Aganemnon </t>
-  </si>
-  <si>
     <t>Opaczny</t>
   </si>
   <si>
@@ -200,55 +188,88 @@
     <t>Olimpijski</t>
   </si>
   <si>
+    <t>Kraków</t>
+  </si>
+  <si>
+    <t>Pacanów</t>
+  </si>
+  <si>
+    <t>ul. Nieistniejąca 2</t>
+  </si>
+  <si>
+    <t>Bżęczyszczykiewicze</t>
+  </si>
+  <si>
+    <t>ul. Niecodłuższa 33/4c</t>
+  </si>
+  <si>
+    <t>ul. Absolutnienajdłuższajakamożeprzejść 44 / 21 A</t>
+  </si>
+  <si>
+    <t>Koniuszowice 7</t>
+  </si>
+  <si>
+    <t>Kataryna@gmail.com</t>
+  </si>
+  <si>
+    <t>maria222@gmail.com</t>
+  </si>
+  <si>
+    <t>monumia@wp.pl</t>
+  </si>
+  <si>
+    <t>Akon990pp@op.pl</t>
+  </si>
+  <si>
+    <t>Demigod@oo.com</t>
+  </si>
+  <si>
+    <t>ul. Krótka 1</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>123 123 123</t>
+  </si>
+  <si>
+    <t>888 888 999</t>
+  </si>
+  <si>
+    <t>320 129 399</t>
+  </si>
+  <si>
+    <t>444 232 421</t>
+  </si>
+  <si>
     <t>31-333</t>
   </si>
   <si>
-    <t>Kraków</t>
-  </si>
-  <si>
     <t>33-311</t>
   </si>
   <si>
-    <t>Pacanów</t>
-  </si>
-  <si>
     <t>11-666</t>
   </si>
   <si>
-    <t>ul. Nieistniejąca 2</t>
-  </si>
-  <si>
-    <t>Bżęczyszczykiewicze</t>
-  </si>
-  <si>
-    <t>ul. Niecodłuższa 33/4c</t>
-  </si>
-  <si>
-    <t>ul. Absolutnienajdłuższajakamożeprzejść 44 / 21 A</t>
-  </si>
-  <si>
-    <t>Koniuszowice 7</t>
+    <t>12-222</t>
   </si>
   <si>
     <t>55-565</t>
   </si>
   <si>
-    <t>Kataryna@gmail.com</t>
-  </si>
-  <si>
-    <t>maria222@gmail.com</t>
-  </si>
-  <si>
-    <t>monumia@wp.pl</t>
-  </si>
-  <si>
-    <t>Akon990pp@op.pl</t>
-  </si>
-  <si>
-    <t>Demigod@oo.com</t>
-  </si>
-  <si>
-    <t>ul. Krótka 1</t>
+    <t>Kataryna</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Aganemnon</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>799 799 799</t>
   </si>
 </sst>
 </file>
@@ -293,18 +314,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -822,7 +840,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,132 +884,132 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="4">
-        <v>123123123</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="4">
-        <v>799799799</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="4">
-        <v>888888999</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="4">
-        <v>320129099</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="4">
-        <v>12222</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D6" s="4">
-        <v>444232421</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1003,5 +1021,6 @@
     <hyperlink ref="A6" r:id="rId5" xr:uid="{883D663E-9FEA-429C-B166-5188591B32FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>